<commit_message>
Added new file + changes
</commit_message>
<xml_diff>
--- a/MSR.xlsx
+++ b/MSR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whmei\Google Drive\Personal\Exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whmei\Desktop\learn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="64">
   <si>
     <t>Rep 1</t>
   </si>
@@ -990,19 +990,19 @@
       </c>
       <c r="C5" s="22">
         <f>Squats!C2</f>
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D5" s="24">
         <f>Squats!F2</f>
-        <v>0.7</v>
+        <v>7.4999999999999956E-2</v>
       </c>
       <c r="E5" s="22">
         <f>Squats!I39</f>
-        <v>2370</v>
+        <v>480</v>
       </c>
       <c r="F5" s="22">
         <f>Squats!I2</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2501,7 +2501,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="N16" sqref="A7:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,7 +2531,7 @@
       <c r="B2" s="34"/>
       <c r="C2" s="18">
         <f>MAX(B5:H38)</f>
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D2" s="34" t="s">
         <v>25</v>
@@ -2539,7 +2539,7 @@
       <c r="E2" s="34"/>
       <c r="F2" s="19">
         <f>(MAX(B5:H38)/MIN(B5)-1)</f>
-        <v>0.7</v>
+        <v>7.4999999999999956E-2</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13" t="s">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="I2" s="5">
         <f>ROUNDUP(MAX(B5:H38)/10,0)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2642,175 +2642,84 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="15">
-        <v>50</v>
-      </c>
-      <c r="C7" s="15">
-        <v>26</v>
-      </c>
-      <c r="D7" s="15">
-        <v>25</v>
-      </c>
-      <c r="E7" s="15">
-        <v>19</v>
-      </c>
+      <c r="A7" s="10"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
-      <c r="I7" s="2">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="15">
-        <v>52</v>
-      </c>
-      <c r="C8" s="15">
-        <v>25</v>
-      </c>
-      <c r="D8" s="15">
-        <v>33</v>
-      </c>
-      <c r="E8" s="15">
-        <v>10</v>
-      </c>
+      <c r="A8" s="10"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
-      <c r="I8" s="2">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="15">
-        <v>45</v>
-      </c>
-      <c r="C9" s="15">
-        <v>29</v>
-      </c>
-      <c r="D9" s="15">
-        <v>30</v>
-      </c>
-      <c r="E9" s="15">
-        <v>31</v>
-      </c>
+      <c r="A9" s="10"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="2">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="15">
-        <v>61</v>
-      </c>
-      <c r="C10" s="15">
-        <v>35</v>
-      </c>
-      <c r="D10" s="15">
-        <v>39</v>
-      </c>
+      <c r="A10" s="10"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
-      <c r="I10" s="2">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="15">
-        <v>68</v>
-      </c>
-      <c r="C11" s="15">
-        <v>41</v>
-      </c>
-      <c r="D11" s="15">
-        <v>26</v>
-      </c>
+      <c r="A11" s="10"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="2">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="15">
-        <v>55</v>
-      </c>
-      <c r="C12" s="15">
-        <v>28</v>
-      </c>
-      <c r="D12" s="15">
-        <v>28</v>
-      </c>
-      <c r="E12" s="15">
-        <v>34</v>
-      </c>
-      <c r="F12" s="15">
-        <v>30</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="2">
-        <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="15">
-        <v>55</v>
-      </c>
-      <c r="C13" s="15">
-        <v>22</v>
-      </c>
-      <c r="D13" s="15">
-        <v>22</v>
-      </c>
-      <c r="E13" s="15">
-        <v>26</v>
-      </c>
+      <c r="A13" s="10"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="2">
-        <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="A14" s="10"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -2818,15 +2727,10 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="A15" s="10"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -2834,15 +2738,10 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="A16" s="10"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -2850,10 +2749,7 @@
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
@@ -3220,7 +3116,7 @@
       <c r="H39" s="38"/>
       <c r="I39" s="21">
         <f>SUM(I5:I38)*2</f>
-        <v>2370</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>